<commit_message>
perbaikan format buku besar
</commit_message>
<xml_diff>
--- a/tbs_template/template_buku_besar.xlsx
+++ b/tbs_template/template_buku_besar.xlsx
@@ -92,7 +92,7 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -116,7 +116,7 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -124,22 +124,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="5"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -203,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -216,11 +201,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,24 +209,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -360,20 +329,20 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="52.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="66.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="9.13"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -384,7 +353,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="8.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -393,7 +362,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -404,7 +373,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -415,120 +384,120 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" s="7" customFormat="true" ht="8.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" s="5" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+    <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" s="7" customFormat="true" ht="8.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" s="12" customFormat="true" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" s="8" customFormat="true" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+    <row r="10" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
perbaikan format laporan buku besar
</commit_message>
<xml_diff>
--- a/tbs_template/template_buku_besar.xlsx
+++ b/tbs_template/template_buku_besar.xlsx
@@ -20,15 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">PD. PEMBANGUNAN SARANA JAYA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">PERUMDA PEMBANGUNAN SARANA JAYA</t>
   </si>
   <si>
     <t xml:space="preserve">Laporan Buku Besar</t>
   </si>
   <si>
-    <t xml:space="preserve">Periode 1 Januari [p.tahun] – [p.bulan] [p.tahun]</t>
+    <t xml:space="preserve">Periode [p.tgawal] s.d. [p.tgakhir]</t>
   </si>
   <si>
     <t xml:space="preserve">Akun : [p.kdakun] - [p.nmakun]</t>
@@ -55,6 +55,18 @@
     <t xml:space="preserve">Saldo</t>
   </si>
   <si>
+    <t xml:space="preserve">Saldo Awal :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[p.sawal_debet]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[p.sawal_kredit]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[p.sawal_saldo]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[v.tanggal]</t>
   </si>
   <si>
@@ -67,19 +79,22 @@
     <t xml:space="preserve">[v.remark;block=tbs:row]</t>
   </si>
   <si>
-    <t xml:space="preserve">[v.debet;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[v.kredit;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[v.saldo;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[p.debet;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[p.kredit;ope=tbs:num]</t>
+    <t xml:space="preserve">[v.debet]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[v.kredit]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[v.saldo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[p.debet]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[p.kredit]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[p.saldo]</t>
   </si>
 </sst>
 </file>
@@ -145,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -158,6 +173,69 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -188,7 +266,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,24 +303,64 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="10" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -326,18 +444,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="66.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="79.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="9.13"/>
   </cols>
@@ -445,59 +563,87 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+    <row r="10" s="8" customFormat="true" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="E10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="G10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="10" t="s">
+    </row>
+    <row r="11" s="15" customFormat="true" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="B11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="E11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="F11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" s="15" customFormat="true" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>